<commit_message>
feat: add plot scripts
</commit_message>
<xml_diff>
--- a/metrics/ext/final_metrics.xlsx
+++ b/metrics/ext/final_metrics.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20413"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\phaxssi\GitHub\Towards_Optimal_RAG\metrics\ext\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3231D76C-0129-4023-A838-E5D7AA25FCB0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Bert Multicased (178M)" sheetId="1" r:id="rId1"/>
-    <sheet name="DistilBERT (65M)" sheetId="2" r:id="rId2"/>
-    <sheet name="RoBERTa (560M)" sheetId="3" r:id="rId3"/>
+    <sheet name="RoBERTa (560M)" sheetId="1" r:id="rId1"/>
+    <sheet name="Bert Multicased (178M)" sheetId="2" r:id="rId2"/>
+    <sheet name="DistilBERT (65M)" sheetId="3" r:id="rId3"/>
     <sheet name="Bert Uncased (335M)" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -67,10 +74,10 @@
     <t>EM - 2V</t>
   </si>
   <si>
-    <t>Cosine</t>
-  </si>
-  <si>
-    <t>Jaccard</t>
+    <t>EM - Cosine (threshold = 0.8)</t>
+  </si>
+  <si>
+    <t>EM - Jaccard (threshold = 0.8)</t>
   </si>
   <si>
     <t>RougeL</t>
@@ -82,8 +89,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,10 +101,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,6 +150,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -433,14 +445,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -481,285 +493,285 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0.5824761904761905</v>
+        <v>0.80406378066378115</v>
       </c>
       <c r="C2">
-        <v>0.1844223684299826</v>
+        <v>6.8277077647905041E-3</v>
       </c>
       <c r="D2">
-        <v>0.5723809523809524</v>
+        <v>0.75554088504088512</v>
       </c>
       <c r="E2">
-        <v>0.08847408885709401</v>
+        <v>2.125597796090354E-2</v>
       </c>
       <c r="F2">
-        <v>0.5310476190476191</v>
+        <v>0.6980239538239541</v>
       </c>
       <c r="G2">
-        <v>0.2104973055558158</v>
+        <v>1.254183590160199E-2</v>
       </c>
       <c r="H2">
-        <v>0.4266666666666666</v>
+        <v>0.63716151996152015</v>
       </c>
       <c r="I2">
-        <v>0.1874037923999824</v>
+        <v>2.3697690719058199E-2</v>
       </c>
       <c r="J2">
-        <v>0.4537142857142857</v>
+        <v>0.56029206349206373</v>
       </c>
       <c r="K2">
-        <v>0.1954732613898058</v>
+        <v>2.2155201087965148E-2</v>
       </c>
       <c r="L2">
-        <v>0.09904761904761904</v>
+        <v>0.13669894179894179</v>
       </c>
       <c r="M2">
-        <v>0.1038051549976283</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>1.082012836183468E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>0.28</v>
+        <v>0.65399999999999991</v>
       </c>
       <c r="C3">
-        <v>0.1095445115010332</v>
+        <v>1.064581294844754E-2</v>
       </c>
       <c r="D3">
-        <v>0.32</v>
+        <v>0.60199999999999998</v>
       </c>
       <c r="E3">
-        <v>0.1095445115010332</v>
+        <v>2.2060522810365722E-2</v>
       </c>
       <c r="F3">
-        <v>0.32</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="G3">
-        <v>0.2280350850198276</v>
+        <v>1.1450376024878471E-2</v>
       </c>
       <c r="H3">
-        <v>0.24</v>
+        <v>0.48799999999999999</v>
       </c>
       <c r="I3">
-        <v>0.1673320053068151</v>
+        <v>2.523225449036743E-2</v>
       </c>
       <c r="J3">
-        <v>0.32</v>
+        <v>0.41333333333333339</v>
       </c>
       <c r="K3">
-        <v>0.1095445115010332</v>
+        <v>2.8674417556808721E-2</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>4.000000000000001E-3</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>2.788866755113585E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0.6799999999999999</v>
+        <v>0.83933333333333326</v>
       </c>
       <c r="C4">
-        <v>0.303315017762062</v>
+        <v>7.9582242575422166E-3</v>
       </c>
       <c r="D4">
-        <v>0.68</v>
+        <v>0.77333333333333332</v>
       </c>
       <c r="E4">
-        <v>0.1095445115010333</v>
+        <v>2.8284271247461901E-2</v>
       </c>
       <c r="F4">
-        <v>0.5600000000000001</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="G4">
-        <v>0.2190890230020665</v>
+        <v>1.615893285805441E-2</v>
       </c>
       <c r="H4">
-        <v>0.4400000000000001</v>
+        <v>0.63066666666666671</v>
       </c>
       <c r="I4">
-        <v>0.260768096208106</v>
+        <v>2.253392504154076E-2</v>
       </c>
       <c r="J4">
-        <v>0.4400000000000001</v>
+        <v>0.53466666666666662</v>
       </c>
       <c r="K4">
-        <v>0.260768096208106</v>
+        <v>3.023978248011126E-2</v>
       </c>
       <c r="L4">
-        <v>0.04</v>
+        <v>2.2666666666666668E-2</v>
       </c>
       <c r="M4">
-        <v>0.08944271909999159</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>5.4772255750516604E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0.6920580667200001</v>
+        <v>0.74933333333333341</v>
       </c>
       <c r="C5">
-        <v>0.1248223646637975</v>
+        <v>1.639783183499844E-2</v>
       </c>
       <c r="D5">
-        <v>0.719715704312</v>
+        <v>0.70866666666666656</v>
       </c>
       <c r="E5">
-        <v>0.06759664602481329</v>
+        <v>1.8648800974265831E-2</v>
       </c>
       <c r="F5">
-        <v>0.697572896472</v>
+        <v>0.65866666666666673</v>
       </c>
       <c r="G5">
-        <v>0.1437075587353153</v>
+        <v>1.7094508539944119E-2</v>
       </c>
       <c r="H5">
-        <v>0.5756333807080001</v>
+        <v>0.59933333333333338</v>
       </c>
       <c r="I5">
-        <v>0.1703980956664931</v>
+        <v>1.441449887362645E-2</v>
       </c>
       <c r="J5">
-        <v>0.6419597506560001</v>
+        <v>0.52866666666666673</v>
       </c>
       <c r="K5">
-        <v>0.09181840193716782</v>
+        <v>2.10290803941167E-2</v>
       </c>
       <c r="L5">
-        <v>0.380864889324</v>
+        <v>0.158</v>
       </c>
       <c r="M5">
-        <v>0.0788893617585839</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>1.3864422895390281E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0.5266666666680001</v>
+        <v>0.66266666666666674</v>
       </c>
       <c r="C6">
-        <v>0.1756258649660946</v>
+        <v>1.115546702045433E-2</v>
       </c>
       <c r="D6">
-        <v>0.5253333333320001</v>
+        <v>0.61066666666666669</v>
       </c>
       <c r="E6">
-        <v>0.09169999394193601</v>
+        <v>2.253392504154076E-2</v>
       </c>
       <c r="F6">
-        <v>0.478666666664</v>
+        <v>0.55800000000000005</v>
       </c>
       <c r="G6">
-        <v>0.2169562167831258</v>
+        <v>9.6032401939252793E-3</v>
       </c>
       <c r="H6">
-        <v>0.375999999996</v>
+        <v>0.49533333333333329</v>
       </c>
       <c r="I6">
-        <v>0.1909973821821301</v>
+        <v>2.5560386016907719E-2</v>
       </c>
       <c r="J6">
-        <v>0.415333333332</v>
+        <v>0.41733333333333328</v>
       </c>
       <c r="K6">
-        <v>0.1711983904376764</v>
+        <v>2.6915505650915161E-2</v>
       </c>
       <c r="L6">
-        <v>0.07199999999999999</v>
+        <v>9.3333333333333341E-3</v>
       </c>
       <c r="M6">
-        <v>0.07563068160475614</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>5.4772255750516613E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0.5699853479853479</v>
+        <v>0.81491929551929587</v>
       </c>
       <c r="C7">
-        <v>0.186747723572892</v>
+        <v>7.0921577142038592E-3</v>
       </c>
       <c r="D7">
-        <v>0.5584615384615386</v>
+        <v>0.77054069264069303</v>
       </c>
       <c r="E7">
-        <v>0.08939308843727814</v>
+        <v>1.6796247537665229E-2</v>
       </c>
       <c r="F7">
-        <v>0.5374212454212455</v>
+        <v>0.71652053872053922</v>
       </c>
       <c r="G7">
-        <v>0.21881243668595</v>
+        <v>1.3753541393586061E-2</v>
       </c>
       <c r="H7">
-        <v>0.4498534798534798</v>
+        <v>0.65189874569874595</v>
       </c>
       <c r="I7">
-        <v>0.1967202808473776</v>
+        <v>2.1112174022591471E-2</v>
       </c>
       <c r="J7">
-        <v>0.5070476190476191</v>
+        <v>0.58230515780515812</v>
       </c>
       <c r="K7">
-        <v>0.1584657162289517</v>
+        <v>2.256854983341396E-2</v>
       </c>
       <c r="L7">
-        <v>0.09238095238095238</v>
+        <v>0.15762914862914859</v>
       </c>
       <c r="M7">
-        <v>0.09231219827364842</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>1.0094160681062239E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0.0339210028144403</v>
+        <v>4.7726098325454477E-2</v>
       </c>
       <c r="C8">
-        <v>0.01896241703951255</v>
+        <v>3.9613805941660649E-3</v>
       </c>
       <c r="D8">
-        <v>0.0339210028144403</v>
+        <v>4.0954971792301037E-2</v>
       </c>
       <c r="E8">
-        <v>0.01896241703951255</v>
+        <v>4.2926788918246682E-3</v>
       </c>
       <c r="F8">
-        <v>0.01696050140722015</v>
+        <v>3.529820384507306E-2</v>
       </c>
       <c r="G8">
-        <v>0.02322412301833147</v>
+        <v>3.855316774538283E-3</v>
       </c>
       <c r="H8">
-        <v>0.008480250703610075</v>
+        <v>3.2062680215039462E-2</v>
       </c>
       <c r="I8">
-        <v>0.01896241703951255</v>
+        <v>4.7266285138500572E-3</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>2.3555013272821251E-2</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>6.3794923663332446E-3</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -769,19 +781,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -822,307 +834,307 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0.5657142857142856</v>
+        <v>0.78345358345358362</v>
       </c>
       <c r="C2">
-        <v>0.1508253934844127</v>
+        <v>7.5155851619479333E-3</v>
       </c>
       <c r="D2">
-        <v>0.5845714285714285</v>
+        <v>0.70520634920634939</v>
       </c>
       <c r="E2">
-        <v>0.1173099853084179</v>
+        <v>1.3207985188359609E-2</v>
       </c>
       <c r="F2">
-        <v>0.5177142857142856</v>
+        <v>0.63591949531949554</v>
       </c>
       <c r="G2">
-        <v>0.1104794744996295</v>
+        <v>1.035971389334862E-2</v>
       </c>
       <c r="H2">
-        <v>0.4323809523809523</v>
+        <v>0.5655894179894182</v>
       </c>
       <c r="I2">
-        <v>0.1151947970606367</v>
+        <v>2.9945215040304531E-2</v>
       </c>
       <c r="J2">
-        <v>0.3788571428571429</v>
+        <v>0.49549255929255942</v>
       </c>
       <c r="K2">
-        <v>0.1415309874485558</v>
+        <v>1.566739909597616E-2</v>
       </c>
       <c r="L2">
-        <v>0.04266666666666667</v>
+        <v>0.1260755466755466</v>
       </c>
       <c r="M2">
-        <v>0.06139127697718046</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>1.354819320950397E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>0.4400000000000001</v>
+        <v>0.60733333333333339</v>
       </c>
       <c r="C3">
-        <v>0.08944271909999157</v>
+        <v>1.9635568633364159E-2</v>
       </c>
       <c r="D3">
-        <v>0.48</v>
+        <v>0.54933333333333334</v>
       </c>
       <c r="E3">
-        <v>0.1095445115010332</v>
+        <v>1.09036181558641E-2</v>
       </c>
       <c r="F3">
-        <v>0.4400000000000001</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="G3">
-        <v>0.08944271909999157</v>
+        <v>8.3666002653407477E-3</v>
       </c>
       <c r="H3">
-        <v>0.36</v>
+        <v>0.41133333333333327</v>
       </c>
       <c r="I3">
-        <v>0.1673320053068151</v>
+        <v>1.894436298451042E-2</v>
       </c>
       <c r="J3">
-        <v>0.28</v>
+        <v>0.35466666666666657</v>
       </c>
       <c r="K3">
-        <v>0.1095445115010332</v>
+        <v>1.5563490039904961E-2</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>2.666666666666667E-3</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>3.651483716701107E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0.4400000000000001</v>
+        <v>0.82400000000000007</v>
       </c>
       <c r="C4">
-        <v>0.08944271909999157</v>
+        <v>7.9582242575422166E-3</v>
       </c>
       <c r="D4">
-        <v>0.52</v>
+        <v>0.72599999999999998</v>
       </c>
       <c r="E4">
-        <v>0.1095445115010332</v>
+        <v>1.588150566609544E-2</v>
       </c>
       <c r="F4">
-        <v>0.4400000000000001</v>
+        <v>0.63400000000000001</v>
       </c>
       <c r="G4">
-        <v>0.08944271909999157</v>
+        <v>1.2337837015547829E-2</v>
       </c>
       <c r="H4">
-        <v>0.4</v>
+        <v>0.54799999999999993</v>
       </c>
       <c r="I4">
-        <v>0.1414213562373095</v>
+        <v>2.9306806187111008E-2</v>
       </c>
       <c r="J4">
-        <v>0.36</v>
+        <v>0.46333333333333337</v>
       </c>
       <c r="K4">
-        <v>0.1673320053068151</v>
+        <v>2.1730674684008831E-2</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>1.8666666666666672E-2</v>
       </c>
       <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>6.4978628965393082E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0.714568372072</v>
+        <v>0.7380000000000001</v>
       </c>
       <c r="C5">
-        <v>0.1202241751529768</v>
+        <v>2.0357908646136621E-2</v>
       </c>
       <c r="D5">
-        <v>0.766031453612</v>
+        <v>0.68066666666666664</v>
       </c>
       <c r="E5">
-        <v>0.07123872143578243</v>
+        <v>1.8012341448141709E-2</v>
       </c>
       <c r="F5">
-        <v>0.704318565732</v>
+        <v>0.60866666666666669</v>
       </c>
       <c r="G5">
-        <v>0.0711281755657463</v>
+        <v>1.0434983894999E-2</v>
       </c>
       <c r="H5">
-        <v>0.582677951304</v>
+        <v>0.55266666666666675</v>
       </c>
       <c r="I5">
-        <v>0.1109793683306803</v>
+        <v>1.4414498873626421E-2</v>
       </c>
       <c r="J5">
-        <v>0.615295473636</v>
+        <v>0.48933333333333329</v>
       </c>
       <c r="K5">
-        <v>0.09271259636274941</v>
+        <v>2.0055478608655111E-2</v>
       </c>
       <c r="L5">
-        <v>0.343415776188</v>
+        <v>0.14133333333333339</v>
       </c>
       <c r="M5">
-        <v>0.05937979561077348</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>2.3285665595430629E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0.532</v>
+        <v>0.61466666666666669</v>
       </c>
       <c r="C6">
-        <v>0.1316054710108968</v>
+        <v>1.8648800974265831E-2</v>
       </c>
       <c r="D6">
-        <v>0.5513333333320001</v>
+        <v>0.55666666666666664</v>
       </c>
       <c r="E6">
-        <v>0.103161146862911</v>
+        <v>9.1287092917527665E-3</v>
       </c>
       <c r="F6">
-        <v>0.492</v>
+        <v>0.48599999999999999</v>
       </c>
       <c r="G6">
-        <v>0.105214067500501</v>
+        <v>9.5452140421842593E-3</v>
       </c>
       <c r="H6">
-        <v>0.412</v>
+        <v>0.41733333333333328</v>
       </c>
       <c r="I6">
-        <v>0.1293058390019569</v>
+        <v>1.8318175552045481E-2</v>
       </c>
       <c r="J6">
-        <v>0.359333333332</v>
+        <v>0.36266666666666658</v>
       </c>
       <c r="K6">
-        <v>0.1296233860911337</v>
+        <v>9.8319208025017413E-3</v>
       </c>
       <c r="L6">
-        <v>0.03000000000000001</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="M6">
-        <v>0.0447213595499958</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>6.9121471177759066E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0.5599999999999999</v>
+        <v>0.78457039257039296</v>
       </c>
       <c r="C7">
-        <v>0.1488847428941819</v>
+        <v>7.6034335945886263E-3</v>
       </c>
       <c r="D7">
-        <v>0.578857142857143</v>
+        <v>0.70977944832944873</v>
       </c>
       <c r="E7">
-        <v>0.1190112325345291</v>
+        <v>1.284537942520626E-2</v>
       </c>
       <c r="F7">
-        <v>0.5148571428571429</v>
+        <v>0.64017272727272767</v>
       </c>
       <c r="G7">
-        <v>0.1124885481699704</v>
+        <v>8.5696130990055332E-3</v>
       </c>
       <c r="H7">
-        <v>0.4295238095238095</v>
+        <v>0.56967633107633131</v>
       </c>
       <c r="I7">
-        <v>0.1144913824005586</v>
+        <v>2.8969344433046738E-2</v>
       </c>
       <c r="J7">
-        <v>0.3693333333333333</v>
+        <v>0.50310322640322647</v>
       </c>
       <c r="K7">
-        <v>0.1376670702173262</v>
+        <v>1.8403406753334541E-2</v>
       </c>
       <c r="L7">
-        <v>0.04266666666666667</v>
+        <v>0.1371115107115107</v>
       </c>
       <c r="M7">
-        <v>0.06139127697718046</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>1.5099076344147439E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>6.2259872659520502E-2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>2.9344185399121491E-3</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>5.0164106161227962E-2</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>5.4609665988248251E-3</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>3.6356067882174083E-2</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>3.9022116474285409E-3</v>
       </c>
       <c r="H8">
-        <v>0.04</v>
+        <v>3.4982330004011193E-2</v>
       </c>
       <c r="I8">
-        <v>0.08944271909999159</v>
+        <v>9.0427541657522575E-3</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>2.664056902804144E-2</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>8.6277597612650723E-3</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>1.55760156614281E-3</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1.421889188969653E-3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1163,285 +1175,285 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0.5662857142857144</v>
+        <v>0.72315694675694708</v>
       </c>
       <c r="C2">
-        <v>0.1152766562795486</v>
+        <v>9.6109418480186844E-3</v>
       </c>
       <c r="D2">
-        <v>0.5634285714285715</v>
+        <v>0.6295299145299148</v>
       </c>
       <c r="E2">
-        <v>0.08763871414898255</v>
+        <v>4.9144173519275009E-3</v>
       </c>
       <c r="F2">
-        <v>0.5862857142857142</v>
+        <v>0.5620860472860475</v>
       </c>
       <c r="G2">
-        <v>0.09279876064541089</v>
+        <v>2.4857879252927682E-2</v>
       </c>
       <c r="H2">
-        <v>0.5737142857142856</v>
+        <v>0.49789259259259272</v>
       </c>
       <c r="I2">
-        <v>0.1051736497352805</v>
+        <v>1.9500487353568349E-2</v>
       </c>
       <c r="J2">
-        <v>0.4619047619047619</v>
+        <v>0.41356560846560858</v>
       </c>
       <c r="K2">
-        <v>0.1410199323329604</v>
+        <v>2.1629041243200892E-2</v>
       </c>
       <c r="L2">
-        <v>0.1714285714285714</v>
+        <v>0.1091084656084656</v>
       </c>
       <c r="M2">
-        <v>0.1118794297568641</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>9.9844977962392587E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>0.36</v>
+        <v>0.55733333333333324</v>
       </c>
       <c r="C3">
-        <v>0.0894427190999916</v>
+        <v>1.622754859285078E-2</v>
       </c>
       <c r="D3">
-        <v>0.36</v>
+        <v>0.47799999999999992</v>
       </c>
       <c r="E3">
-        <v>0.08944271909999159</v>
+        <v>6.4978628965393342E-3</v>
       </c>
       <c r="F3">
-        <v>0.4399999999999999</v>
+        <v>0.42066666666666669</v>
       </c>
       <c r="G3">
-        <v>0.1673320053068151</v>
+        <v>3.402613374713289E-2</v>
       </c>
       <c r="H3">
-        <v>0.4</v>
+        <v>0.36599999999999999</v>
       </c>
       <c r="I3">
-        <v>0.1414213562373095</v>
+        <v>1.5705625319186331E-2</v>
       </c>
       <c r="J3">
-        <v>0.28</v>
+        <v>0.27933333333333338</v>
       </c>
       <c r="K3">
-        <v>0.1095445115010332</v>
+        <v>2.691550565091512E-2</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>4.3461349368017661E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0.6</v>
+        <v>0.7433333333333334</v>
       </c>
       <c r="C4">
-        <v>0.1414213562373095</v>
+        <v>1.224744871391591E-2</v>
       </c>
       <c r="D4">
-        <v>0.6399999999999999</v>
+        <v>0.64133333333333331</v>
       </c>
       <c r="E4">
-        <v>0.08944271909999162</v>
+        <v>8.6922698736035323E-3</v>
       </c>
       <c r="F4">
-        <v>0.6000000000000001</v>
+        <v>0.54333333333333333</v>
       </c>
       <c r="G4">
-        <v>0.1414213562373095</v>
+        <v>3.3582402799349813E-2</v>
       </c>
       <c r="H4">
-        <v>0.6</v>
+        <v>0.47</v>
       </c>
       <c r="I4">
-        <v>0.1414213562373095</v>
+        <v>2.2236106773543901E-2</v>
       </c>
       <c r="J4">
-        <v>0.52</v>
+        <v>0.37666666666666659</v>
       </c>
       <c r="K4">
-        <v>0.1095445115010332</v>
+        <v>1.50923085635624E-2</v>
       </c>
       <c r="L4">
-        <v>0.12</v>
+        <v>1.1333333333333339E-2</v>
       </c>
       <c r="M4">
-        <v>0.1095445115010332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>5.0552502960343687E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0.6791031458879999</v>
+        <v>0.67666666666666664</v>
       </c>
       <c r="C5">
-        <v>0.07523185072929545</v>
+        <v>1.9860625479688299E-2</v>
       </c>
       <c r="D5">
-        <v>0.7112814950840001</v>
+        <v>0.60599999999999998</v>
       </c>
       <c r="E5">
-        <v>0.04640637527137942</v>
+        <v>1.1879019787470279E-2</v>
       </c>
       <c r="F5">
-        <v>0.7675087529360001</v>
+        <v>0.54200000000000004</v>
       </c>
       <c r="G5">
-        <v>0.1050627995079629</v>
+        <v>3.3132729706104487E-2</v>
       </c>
       <c r="H5">
-        <v>0.8093880236040001</v>
+        <v>0.4913333333333334</v>
       </c>
       <c r="I5">
-        <v>0.05479163956130314</v>
+        <v>2.4106246309019391E-2</v>
       </c>
       <c r="J5">
-        <v>0.7443953430520001</v>
+        <v>0.41399999999999998</v>
       </c>
       <c r="K5">
-        <v>0.05174569215506118</v>
+        <v>4.1190613817551541E-2</v>
       </c>
       <c r="L5">
-        <v>0.41283599882</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="M5">
-        <v>0.08996193250104863</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>2.40831891575846E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0.473333333328</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="C6">
-        <v>0.1307244770091321</v>
+        <v>1.8104634152000362E-2</v>
       </c>
       <c r="D6">
-        <v>0.477333333328</v>
+        <v>0.48666666666666669</v>
       </c>
       <c r="E6">
-        <v>0.0961017978782453</v>
+        <v>6.2360956446232156E-3</v>
       </c>
       <c r="F6">
-        <v>0.5439999999999999</v>
+        <v>0.43</v>
       </c>
       <c r="G6">
-        <v>0.1069631296856798</v>
+        <v>3.1972210155418138E-2</v>
       </c>
       <c r="H6">
-        <v>0.522</v>
+        <v>0.36999999999999988</v>
       </c>
       <c r="I6">
-        <v>0.109888832714602</v>
+        <v>1.3333333333333339E-2</v>
       </c>
       <c r="J6">
-        <v>0.394666666664</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K6">
-        <v>0.1328658471277953</v>
+        <v>2.7487370837451099E-2</v>
       </c>
       <c r="L6">
-        <v>0.124</v>
+        <v>6.6666666666666662E-3</v>
       </c>
       <c r="M6">
-        <v>0.0817312669668102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>4.7140452079103149E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0.6005714285714285</v>
+        <v>0.71783138528138557</v>
       </c>
       <c r="C7">
-        <v>0.09052905723623567</v>
+        <v>1.1385593625652441E-2</v>
       </c>
       <c r="D7">
-        <v>0.6376623376623376</v>
+        <v>0.62964027454027482</v>
       </c>
       <c r="E7">
-        <v>0.06335431650340467</v>
+        <v>5.6528073641658608E-3</v>
       </c>
       <c r="F7">
-        <v>0.638996336996337</v>
+        <v>0.56239980759980779</v>
       </c>
       <c r="G7">
-        <v>0.08803163270064904</v>
+        <v>2.474979204203721E-2</v>
       </c>
       <c r="H7">
-        <v>0.6698967698967699</v>
+        <v>0.50264660894660906</v>
       </c>
       <c r="I7">
-        <v>0.05625610808585568</v>
+        <v>1.965829690913605E-2</v>
       </c>
       <c r="J7">
-        <v>0.6485714285714286</v>
+        <v>0.4181931660931662</v>
       </c>
       <c r="K7">
-        <v>0.03056534578263089</v>
+        <v>2.4046270450408452E-2</v>
       </c>
       <c r="L7">
-        <v>0.1514285714285714</v>
+        <v>0.1229302364302364</v>
       </c>
       <c r="M7">
-        <v>0.09508320738453564</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>1.064750040945202E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>5.7903539873154393E-2</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>4.3384887455711497E-3</v>
       </c>
       <c r="D8">
-        <v>0.01050763957769663</v>
+        <v>4.5492267743045253E-2</v>
       </c>
       <c r="E8">
-        <v>0.02349579637879685</v>
+        <v>7.5517379682322394E-3</v>
       </c>
       <c r="F8">
-        <v>0.008480250703610075</v>
+        <v>2.9258881804465689E-2</v>
       </c>
       <c r="G8">
-        <v>0.01896241703951255</v>
+        <v>4.9306057702343826E-3</v>
       </c>
       <c r="H8">
-        <v>0.01898789028130671</v>
+        <v>2.8468337099663659E-2</v>
       </c>
       <c r="I8">
-        <v>0.02624608852094292</v>
+        <v>4.5247406347660533E-3</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>1.6270422170220511E-2</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>5.6440967666509011E-3</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1451,19 +1463,19 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1504,294 +1516,294 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
       <c r="B2">
-        <v>0.6746666666666666</v>
+        <v>0.78691986161986194</v>
       </c>
       <c r="C2">
-        <v>0.1699934639266398</v>
+        <v>1.425905624944401E-2</v>
       </c>
       <c r="D2">
-        <v>0.639904761904762</v>
+        <v>0.72657277167277212</v>
       </c>
       <c r="E2">
-        <v>0.1752149311812311</v>
+        <v>1.392717049699879E-2</v>
       </c>
       <c r="F2">
-        <v>0.6144761904761904</v>
+        <v>0.66203663003663027</v>
       </c>
       <c r="G2">
-        <v>0.09822783456329068</v>
+        <v>1.8926811817164869E-2</v>
       </c>
       <c r="H2">
-        <v>0.709047619047619</v>
+        <v>0.60407513227513243</v>
       </c>
       <c r="I2">
-        <v>0.07879621524803694</v>
+        <v>3.045078907016463E-2</v>
       </c>
       <c r="J2">
-        <v>0.5262857142857144</v>
+        <v>0.5260902319902323</v>
       </c>
       <c r="K2">
-        <v>0.1160823071825174</v>
+        <v>8.5118624806825739E-3</v>
       </c>
       <c r="L2">
-        <v>0.115047619047619</v>
+        <v>0.1622857142857142</v>
       </c>
       <c r="M2">
-        <v>0.02178434812266025</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>1.7429938398701009E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
-        <v>0.36</v>
+        <v>0.6206666666666667</v>
       </c>
       <c r="C3">
-        <v>0.1673320053068151</v>
+        <v>1.9061304607327752E-2</v>
       </c>
       <c r="D3">
-        <v>0.36</v>
+        <v>0.58133333333333337</v>
       </c>
       <c r="E3">
-        <v>0.08944271909999159</v>
+        <v>1.282358937444756E-2</v>
       </c>
       <c r="F3">
-        <v>0.4</v>
+        <v>0.52333333333333332</v>
       </c>
       <c r="G3">
-        <v>0.1414213562373095</v>
+        <v>2.4608038433722359E-2</v>
       </c>
       <c r="H3">
-        <v>0.4399999999999999</v>
+        <v>0.46000000000000008</v>
       </c>
       <c r="I3">
-        <v>0.08944271909999157</v>
+        <v>1.2692955176439801E-2</v>
       </c>
       <c r="J3">
-        <v>0.32</v>
+        <v>0.38933333333333342</v>
       </c>
       <c r="K3">
-        <v>0.1095445115010332</v>
+        <v>1.211060141638994E-2</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="M3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
+        <v>4.9441323247304417E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
       <c r="B4">
-        <v>0.8</v>
+        <v>0.82333333333333347</v>
       </c>
       <c r="C4">
-        <v>0.1414213562373095</v>
+        <v>2.0138409955990959E-2</v>
       </c>
       <c r="D4">
-        <v>0.6799999999999999</v>
+        <v>0.74599999999999989</v>
       </c>
       <c r="E4">
-        <v>0.2280350850198276</v>
+        <v>1.622754859285078E-2</v>
       </c>
       <c r="F4">
-        <v>0.6</v>
+        <v>0.65866666666666673</v>
       </c>
       <c r="G4">
-        <v>0.1414213562373095</v>
+        <v>1.89443629845104E-2</v>
       </c>
       <c r="H4">
-        <v>0.7200000000000001</v>
+        <v>0.58266666666666667</v>
       </c>
       <c r="I4">
-        <v>0.1095445115010333</v>
+        <v>2.2035325174717912E-2</v>
       </c>
       <c r="J4">
-        <v>0.6</v>
+        <v>0.48266666666666658</v>
       </c>
       <c r="K4">
-        <v>0.1414213562373095</v>
+        <v>1.090361815586411E-2</v>
       </c>
       <c r="L4">
-        <v>0.08</v>
+        <v>2.4E-2</v>
       </c>
       <c r="M4">
-        <v>0.1095445115010332</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>6.4117946872237807E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>16</v>
       </c>
       <c r="B5">
-        <v>0.762078136496</v>
+        <v>0.7426666666666667</v>
       </c>
       <c r="C5">
-        <v>0.1653369696617113</v>
+        <v>1.6397831834998461E-2</v>
       </c>
       <c r="D5">
-        <v>0.728877332196</v>
+        <v>0.69266666666666676</v>
       </c>
       <c r="E5">
-        <v>0.07933271053523025</v>
+        <v>1.754359648925434E-2</v>
       </c>
       <c r="F5">
-        <v>0.7617188954280001</v>
+        <v>0.63533333333333331</v>
       </c>
       <c r="G5">
-        <v>0.07369140948294638</v>
+        <v>2.9306806187111002E-2</v>
       </c>
       <c r="H5">
-        <v>0.7924970459839999</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="I5">
-        <v>0.08041947394359544</v>
+        <v>3.0605010483034718E-2</v>
       </c>
       <c r="J5">
-        <v>0.65329677462</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="K5">
-        <v>0.1142841830378465</v>
+        <v>1.7224014243685099E-2</v>
       </c>
       <c r="L5">
-        <v>0.4103990721760001</v>
+        <v>0.184</v>
       </c>
       <c r="M5">
-        <v>0.0718922326983773</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>1.7857460314638519E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
       <c r="B6">
-        <v>0.5933333333319999</v>
+        <v>0.6286666666666666</v>
       </c>
       <c r="C6">
-        <v>0.1718364855890299</v>
+        <v>1.8043158136965821E-2</v>
       </c>
       <c r="D6">
-        <v>0.5570476190440001</v>
+        <v>0.58866666666666667</v>
       </c>
       <c r="E6">
-        <v>0.157073722163721</v>
+        <v>8.6922698736035496E-3</v>
       </c>
       <c r="F6">
-        <v>0.5599999999999999</v>
+        <v>0.52533333333333343</v>
       </c>
       <c r="G6">
-        <v>0.09919117344188329</v>
+        <v>2.3640830968662849E-2</v>
       </c>
       <c r="H6">
-        <v>0.6277142857119999</v>
+        <v>0.46666666666666667</v>
       </c>
       <c r="I6">
-        <v>0.07798002535639634</v>
+        <v>1.433720877840435E-2</v>
       </c>
       <c r="J6">
-        <v>0.470666666664</v>
+        <v>0.39866666666666672</v>
       </c>
       <c r="K6">
-        <v>0.1050502525289894</v>
+        <v>1.6261747890200601E-2</v>
       </c>
       <c r="L6">
-        <v>0.08199999999999999</v>
+        <v>1.1333333333333331E-2</v>
       </c>
       <c r="M6">
-        <v>0.0204939015319192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>8.0277297191948642E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>18</v>
       </c>
       <c r="B7">
-        <v>0.6806060606060605</v>
+        <v>0.78881372331372379</v>
       </c>
       <c r="C7">
-        <v>0.1880082642811653</v>
+        <v>1.546452339721891E-2</v>
       </c>
       <c r="D7">
-        <v>0.636995670995671</v>
+        <v>0.72709005439005492</v>
       </c>
       <c r="E7">
-        <v>0.1721242051618138</v>
+        <v>1.412996439160696E-2</v>
       </c>
       <c r="F7">
-        <v>0.6080872460872461</v>
+        <v>0.66458767713767752</v>
       </c>
       <c r="G7">
-        <v>0.100219548736925</v>
+        <v>2.133474284642644E-2</v>
       </c>
       <c r="H7">
-        <v>0.7274718614718615</v>
+        <v>0.60808715358715393</v>
       </c>
       <c r="I7">
-        <v>0.05656512684912616</v>
+        <v>3.0597459308669559E-2</v>
       </c>
       <c r="J7">
-        <v>0.5352813852813852</v>
+        <v>0.53343885743885777</v>
       </c>
       <c r="K7">
-        <v>0.09495308593761205</v>
+        <v>7.0939492268213226E-3</v>
       </c>
       <c r="L7">
-        <v>0.1017142857142857</v>
+        <v>0.1768232804232803</v>
       </c>
       <c r="M7">
-        <v>0.01408429433584713</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
+        <v>1.382006434480107E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8">
-        <v>0.03581695075211787</v>
+        <v>6.9976707252670106E-2</v>
       </c>
       <c r="C8">
-        <v>0.03269625311331097</v>
+        <v>5.2987444092394004E-3</v>
       </c>
       <c r="D8">
-        <v>0.01193898358403929</v>
+        <v>5.0529739335781428E-2</v>
       </c>
       <c r="E8">
-        <v>0.02669637887616593</v>
+        <v>6.3673739748208854E-3</v>
       </c>
       <c r="F8">
-        <v>0.02041923428764936</v>
+        <v>3.7645611454918702E-2</v>
       </c>
       <c r="G8">
-        <v>0.02862090093328385</v>
+        <v>6.158165733386625E-3</v>
       </c>
       <c r="H8">
-        <v>0.01193898358403929</v>
+        <v>3.5487330537937768E-2</v>
       </c>
       <c r="I8">
-        <v>0.02669637887616593</v>
+        <v>4.8264292946128204E-3</v>
       </c>
       <c r="J8">
-        <v>0.01193898358403929</v>
+        <v>3.1875438485282348E-2</v>
       </c>
       <c r="K8">
-        <v>0.02669637887616593</v>
+        <v>3.5811590857930558E-3</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>5.1920052204760322E-4</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>1.1609676612518191E-3</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>